<commit_message>
Expense and team member pages
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/TestData/testData_Excel.xlsx
+++ b/QA_Legend/src/main/java/TestData/testData_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arun\eclipse-workspace\QA_Legend\src\main\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arun\git\Project-CRM\QA_Legend\src\main\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5725D230-3AF0-4D2B-805C-2E2C603F293E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853FA76-875D-48C2-82AC-D93616E1D074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>selenium testng</t>
   </si>
@@ -76,16 +76,84 @@
   </si>
   <si>
     <t>Electronics</t>
+  </si>
+  <si>
+    <t>Member Firstname</t>
+  </si>
+  <si>
+    <t>Member lastname</t>
+  </si>
+  <si>
+    <t>Member address</t>
+  </si>
+  <si>
+    <t>Harsha</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>harshaarun@mailinator.com</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Job title</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Salary term</t>
+  </si>
+  <si>
+    <t>per month</t>
+  </si>
+  <si>
+    <t>member emailId</t>
+  </si>
+  <si>
+    <t>member password</t>
+  </si>
+  <si>
+    <t>harsha12345</t>
+  </si>
+  <si>
+    <t>Expense Title</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Expense Description</t>
+  </si>
+  <si>
+    <t>traning fees</t>
+  </si>
+  <si>
+    <t>Expense Amount</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,17 +176,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,18 +468,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,7 +551,95 @@
         <v>55000</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>471234535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>25000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1" xr:uid="{E811555D-5CE8-442F-BD05-31AAD3442079}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{7DF5D112-D84B-4C26-A63F-E97DE7FFCDD8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>